<commit_message>
excel sheet with cosine similarity
</commit_message>
<xml_diff>
--- a/with_cosine_similarities.xlsx
+++ b/with_cosine_similarities.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,45 +446,40 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>verb</t>
+          <t>sentence</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>sentence</t>
+          <t>verb_idx</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>verb_idx</t>
+          <t>label</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>label</t>
+          <t>word_1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>word_1</t>
+          <t>word_2</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>word_2</t>
+          <t>word_3</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>word_3</t>
+          <t>CosineSimilarity_1</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>CosineSimilarity_1</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>CosineSimilarity_2</t>
         </is>
@@ -522,7 +517,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>absord</t>
+          <t>absorb</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -530,12 +525,11 @@
           <t>knowledge</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>0.2566680819897257</v>
+      </c>
       <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
+        <v>0.3566897535651615</v>
       </c>
     </row>
     <row r="3">
@@ -578,12 +572,11 @@
           <t>costs</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>0.2566680819897257</v>
+      </c>
       <c r="K3" t="n">
         <v>0.5655341993882779</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -626,12 +619,11 @@
           <t>tax</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>0.3328949117932137</v>
+      </c>
       <c r="K4" t="n">
         <v>0.3328949117932137</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -674,12 +666,11 @@
           <t>society</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>0.4044853740991907</v>
+      </c>
       <c r="K5" t="n">
         <v>0.2710425393070768</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -722,12 +713,11 @@
           <t>interest</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>0.2566680819897257</v>
+      </c>
       <c r="K6" t="n">
         <v>0.4620813639364078</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -770,11 +760,10 @@
           <t xml:space="preserve">person </t>
         </is>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="n">
+        <v>0.2566680819897257</v>
+      </c>
       <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -818,11 +807,10 @@
           <t>system</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
       <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -866,11 +854,10 @@
           <t xml:space="preserve">person </t>
         </is>
       </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
       <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -914,11 +901,10 @@
           <t>alcohol</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
       <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -962,12 +948,11 @@
           <t>people</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>0.4652179322409485</v>
+      </c>
       <c r="K11" t="n">
         <v>0.5271750183652546</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1010,12 +995,11 @@
           <t>results</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>0.5271750183652546</v>
+      </c>
       <c r="K12" t="n">
         <v>0.2160821979520844</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1058,12 +1042,11 @@
           <t>submission</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>0.4385774836555155</v>
+      </c>
       <c r="K13" t="n">
         <v>0.3492648972773089</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1106,12 +1089,11 @@
           <t>people</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>0.4393237764209459</v>
+      </c>
       <c r="K14" t="n">
         <v>0.5605017618147151</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1154,12 +1136,11 @@
           <t>kindness</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>0.5605017618147151</v>
+      </c>
       <c r="K15" t="n">
         <v>0.3398623769483824</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1202,11 +1183,10 @@
           <t>""</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>0.2428670676060369</v>
+      </c>
       <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1250,12 +1230,11 @@
           <t>heir</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>0.4393237764209459</v>
+      </c>
       <c r="K17" t="n">
         <v>0.2068151976367784</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1298,12 +1277,11 @@
           <t>religion</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>0.3408840893203698</v>
+      </c>
       <c r="K18" t="n">
         <v>0.5283742105256388</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1346,12 +1324,11 @@
           <t>wall</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>0.1903674402165263</v>
+      </c>
       <c r="K19" t="n">
         <v>0.08354157338912775</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1394,12 +1371,11 @@
           <t>touch</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="n">
+        <v>0.3722225428879729</v>
+      </c>
       <c r="K20" t="n">
         <v>0.6955257109994322</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1442,11 +1418,10 @@
           <t>""</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="n">
+        <v>0.5664358014308725</v>
+      </c>
       <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1490,12 +1465,11 @@
           <t>answer</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr"/>
+      <c r="J22" t="n">
+        <v>0.8241897019010316</v>
+      </c>
       <c r="K22" t="n">
         <v>0.7281898973172681</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1538,12 +1512,11 @@
           <t>charges</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="n">
+        <v>0.5089019823454131</v>
+      </c>
       <c r="K23" t="n">
         <v>0.5108451962195149</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1586,12 +1559,11 @@
           <t>mountain</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>0.1023919432080509</v>
+      </c>
       <c r="K24" t="n">
         <v>0.4013323617022618</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1634,12 +1606,11 @@
           <t>linearly</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>0.2169892474520203</v>
+      </c>
       <c r="K25" t="n">
         <v>0.1256868588701296</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1682,12 +1653,11 @@
           <t>hill</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr"/>
+      <c r="J26" t="n">
+        <v>0.3949646915641254</v>
+      </c>
       <c r="K26" t="n">
         <v>0.2113993625174003</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1730,12 +1700,11 @@
           <t>country</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr"/>
+      <c r="J27" t="n">
+        <v>0.4925992310255374</v>
+      </c>
       <c r="K27" t="n">
         <v>0.51716012701194</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1778,11 +1747,10 @@
           <t xml:space="preserve">person </t>
         </is>
       </c>
-      <c r="J28" t="inlineStr"/>
+      <c r="J28" t="n">
+        <v>0.104213559963506</v>
+      </c>
       <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1826,12 +1794,11 @@
           <t>problem</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr"/>
+      <c r="J29" t="n">
+        <v>0.4925992310255374</v>
+      </c>
       <c r="K29" t="n">
         <v>0.4752230991641072</v>
-      </c>
-      <c r="L29" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1874,12 +1841,11 @@
           <t>liver</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr"/>
+      <c r="J30" t="n">
+        <v>0.3103177150743683</v>
+      </c>
       <c r="K30" t="n">
         <v>0.1709367300599205</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>